<commit_message>
Updated material profiles Excel sheet
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\3D Printing\manuals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D31BD1-BE19-4B8E-9D08-08CEE3AFC528}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F398E57-A0BB-40AD-A3EA-3A5D819FA747}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Material</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>rigid.ink PLA+</t>
+  </si>
+  <si>
+    <t>MK3 Pretty PETG V2 rigid.ink</t>
+  </si>
+  <si>
+    <t>MK3 Pretty PETG V2 PrimaSelect</t>
+  </si>
+  <si>
+    <t>EasyWood PLA</t>
   </si>
 </sst>
 </file>
@@ -567,12 +576,13 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
   </cols>
@@ -666,6 +676,12 @@
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -687,14 +703,30 @@
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added HIPS profiles and altered PLA profiles for better print reliabliity
Started using the purge bubble methodology with the PLA profile, this seems to work better because of the new Prusa Z probing methodology, as it seems more sensitive to small bits of material on the nozzle. Also added HIPS profile.
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E765EA-151A-46B1-9E72-0439002EE2ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688F89DC-6E79-4338-941C-656C93A49B4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Material</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>rigid.ink HIPS</t>
+  </si>
+  <si>
+    <t>Not quite happy with print quality, oozey and stringy</t>
+  </si>
+  <si>
+    <t>Original Prusa i3 MK3 purgebubble</t>
   </si>
 </sst>
 </file>
@@ -588,14 +594,14 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="142.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -711,7 +717,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -734,8 +740,8 @@
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
+      <c r="B10" t="s">
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -743,7 +749,9 @@
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">

</xml_diff>

<commit_message>
Created Taulman T-Glase profiles
Created Taulman T-Glase profiles in accordance to guidance from Taulman, the Slic3r T-Glase material profile was incorrect
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688F89DC-6E79-4338-941C-656C93A49B4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5763F328-AFCF-43EF-AFFD-355A7DE6025E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Material</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Original Prusa i3 MK3 purgebubble</t>
+  </si>
+  <si>
+    <t>Taulman T-Glase</t>
+  </si>
+  <si>
+    <t>Standard Slic3r profile for T-Glase is nonsense, bed temperature above the glass transition for the material? ¯\_(ツ)_/¯ Generated new profile using guidance from Taulman, and a bit of trial and error</t>
+  </si>
+  <si>
+    <t>Taulman T-Glase mod</t>
   </si>
 </sst>
 </file>
@@ -591,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8993357-4930-402C-A23E-E4B9A1301062}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +611,7 @@
     <col min="1" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="142.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="181.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -738,67 +747,84 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added better logging in sliced gcode files
I was struggling to remember which material profile I used for which particular material. So if you open the .gcode file with a text editor (I recommend Notepad++) it will now have at the top of the .gcode file which print, filament and printer profiles were used to slice that particular file.
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F09EA9-DB3F-454C-8A3A-8EA1B1280B04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEC162C-B0A9-4632-BE6A-29E4F85BDBBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t>Material</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Graphene Enhanced PLA</t>
   </si>
   <si>
-    <t>Protopast Conductive</t>
-  </si>
-  <si>
     <t>Slight artifacts on overhangs</t>
   </si>
   <si>
@@ -154,6 +151,39 @@
   </si>
   <si>
     <t xml:space="preserve">Prints good, colour not nearly as vivid when compared to rigid.ink, I have only used orange. </t>
+  </si>
+  <si>
+    <t>rigid.ink ABS Ultra Durable</t>
+  </si>
+  <si>
+    <t>FilaPrint PETG</t>
+  </si>
+  <si>
+    <t>MK3 Pretty PETG V2 filaprint</t>
+  </si>
+  <si>
+    <t>Protopasta Conductive</t>
+  </si>
+  <si>
+    <t>Proto-pasta HTPLA Matte Fibre</t>
+  </si>
+  <si>
+    <t>Fillamentum PLA Extrafill</t>
+  </si>
+  <si>
+    <t>Consistent, light stringing, first layer 240°C to break nozzle blockage, further layers 210, could potentially go lower.</t>
+  </si>
+  <si>
+    <t>Need to dry filament before assessing print quality.</t>
+  </si>
+  <si>
+    <t>igus iglidur I150</t>
+  </si>
+  <si>
+    <t>iglidur I150</t>
+  </si>
+  <si>
+    <t>First one came out with some moderate blistering and some stringing, reduce extrusion multiplier and increase cooling?</t>
   </si>
 </sst>
 </file>
@@ -643,16 +673,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8993357-4930-402C-A23E-E4B9A1301062}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="181.42578125" bestFit="1" customWidth="1"/>
@@ -682,7 +711,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -694,7 +723,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,26 +745,26 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
@@ -744,45 +773,43 @@
       <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -790,181 +817,265 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
+      <c r="A11" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
+      <c r="A12" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
+      <c r="A13" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>17</v>
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C22" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B23" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C23" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D23" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="E23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:E19">
-    <sortCondition ref="A3:A19"/>
+  <sortState ref="A3:E24">
+    <sortCondition ref="A3:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ABS Ultra Durable profile
Updated ABS Ultra Durable profile for better performance, tested with enclosure only.
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB84099F-A255-4354-879D-C8535F41606C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6110CF2A-4129-47C4-AA24-F36D69191162}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="44">
   <si>
     <t>Material</t>
   </si>
@@ -540,9 +540,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>No, but would probably be helpful</t>
   </si>
   <si>
     <t>READ THE NOTES IN COLUMN D</t>
@@ -1120,7 +1117,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1131,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1159,10 +1156,10 @@
         <v>37</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1407,10 +1404,10 @@
         <v>7</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G17" s="2"/>
     </row>
@@ -1428,9 +1425,11 @@
         <v>7</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>43</v>
+      </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,10 +1446,10 @@
         <v>7</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G19" s="2"/>
     </row>
@@ -1487,10 +1486,10 @@
         <v>7</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="2"/>
     </row>

</xml_diff>

<commit_message>
Updated a number of profiles
Updated the rigid.ink Nylon 12 profile, pretty happy with this one now. Added profiles for the iglidur I150-PF material, which is a low friction bearing material, added profiles for Filaprint PETG and Proto-pasta HTPLA as well as rigid.inks Ultra Durable ABS, an ABS Nylon blend.
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6110CF2A-4129-47C4-AA24-F36D69191162}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA337B47-3942-482D-BAFE-53629B8E472F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
   <si>
     <t>Material</t>
   </si>
@@ -555,6 +555,21 @@
   </si>
   <si>
     <t>Brim useful depending on shape</t>
+  </si>
+  <si>
+    <t>Stringy</t>
+  </si>
+  <si>
+    <t>Stringy, but cleans up fine</t>
+  </si>
+  <si>
+    <t>Stringy, but cleans up pretty well</t>
+  </si>
+  <si>
+    <t>Not great quality</t>
+  </si>
+  <si>
+    <t>Quite blobby, cleans up well</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1132,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1231,9 @@
       <c r="E7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1368,7 +1385,9 @@
       <c r="E15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1387,7 +1406,9 @@
       <c r="E16" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="11"/>
+      <c r="F16" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1469,7 +1490,9 @@
       <c r="E20" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="11"/>
+      <c r="F20" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1547,7 +1570,9 @@
       <c r="E24" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="11"/>
+      <c r="F24" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1566,7 +1591,9 @@
       <c r="E25" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="11"/>
+      <c r="F25" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Included Taulman Bridge profile
Included Taulman Bridge profile and updated spreadsheet
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA337B47-3942-482D-BAFE-53629B8E472F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC43634-4305-41F0-929D-A9BDFB3DF438}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -394,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
       <text>
         <r>
           <rPr>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="52">
   <si>
     <t>Material</t>
   </si>
@@ -570,6 +570,15 @@
   </si>
   <si>
     <t>Quite blobby, cleans up well</t>
+  </si>
+  <si>
+    <t>Taulman Bridge</t>
+  </si>
+  <si>
+    <t>Taulman Bridge mod</t>
+  </si>
+  <si>
+    <t>Tiny bit of stringing, thin layer of glue stick required</t>
   </si>
 </sst>
 </file>
@@ -1129,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8993357-4930-402C-A23E-E4B9A1301062}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1149,8 @@
     <col min="1" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1597,27 +1607,48 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
+      <c r="E27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A5:E26">
-    <sortCondition ref="A5:A26"/>
+  <sortState ref="A5:E27">
+    <sortCondition ref="A5:A27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Fillamentum CPE profile
Made minimal changes to the Prusa standard profile, just slowed things down to get reliable prints.
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674D131C-BA09-46B1-85B1-958C860E6A86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DCA764-4832-474F-A311-03CA545B26FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -106,7 +106,7 @@
     <comment ref="F7" authorId="0" shapeId="0" xr:uid="{221044AA-A390-4D84-BA7C-0914AFFBB821}">
       <text/>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{A8745309-D847-4CF9-A000-C21A4470BCE6}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{B2EAE4EC-6C25-4511-9920-3BC8F3F2B3B6}">
       <text>
         <r>
           <rPr>
@@ -126,11 +126,36 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
+First print came out really well, I have just changed things like minimum speeds and minimum layer times to improve reliability. No brim used but slight warping was seen on Benchy base.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{A8745309-D847-4CF9-A000-C21A4470BCE6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darragh Broadbent:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 A very small amount of discolouration on one of the pillars</t>
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{985DE15F-4A11-41B1-8852-8A4820DB9028}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{985DE15F-4A11-41B1-8852-8A4820DB9028}">
       <text>
         <r>
           <rPr>
@@ -154,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{54BD3F34-1376-445B-88F8-B91899B9F727}">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{54BD3F34-1376-445B-88F8-B91899B9F727}">
       <text>
         <r>
           <rPr>
@@ -178,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{6CD30595-BA02-485E-9C00-1233A05C83DE}">
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{6CD30595-BA02-485E-9C00-1233A05C83DE}">
       <text>
         <r>
           <rPr>
@@ -202,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{6FD53F9C-5A10-4655-B410-C14919F7F484}">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{6FD53F9C-5A10-4655-B410-C14919F7F484}">
       <text>
         <r>
           <rPr>
@@ -226,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{7F30C7B6-B556-4FF9-B1F0-6CB901BE9E8C}">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{7F30C7B6-B556-4FF9-B1F0-6CB901BE9E8C}">
       <text>
         <r>
           <rPr>
@@ -250,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{D5CE3906-B1F3-484F-937A-234E258807EE}">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{D5CE3906-B1F3-484F-937A-234E258807EE}">
       <text>
         <r>
           <rPr>
@@ -274,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{E0462C9B-BC3A-4A76-8CFA-B66364D1B3ED}">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{E0462C9B-BC3A-4A76-8CFA-B66364D1B3ED}">
       <text>
         <r>
           <rPr>
@@ -298,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{ECE11F64-1683-473C-9AC3-F116D9ED5E60}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{ECE11F64-1683-473C-9AC3-F116D9ED5E60}">
       <text>
         <r>
           <rPr>
@@ -322,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{0023CEED-8BBE-4786-A3A8-FF9F7051A736}">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{0023CEED-8BBE-4786-A3A8-FF9F7051A736}">
       <text>
         <r>
           <rPr>
@@ -347,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{B0295431-8909-4919-8B34-7A07B2F464CD}">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{B0295431-8909-4919-8B34-7A07B2F464CD}">
       <text>
         <r>
           <rPr>
@@ -372,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{FA5AB986-6F3D-4095-AA62-83099A764AA8}">
+    <comment ref="D26" authorId="0" shapeId="0" xr:uid="{FA5AB986-6F3D-4095-AA62-83099A764AA8}">
       <text>
         <r>
           <rPr>
@@ -396,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="0" shapeId="0" xr:uid="{8CF096DE-B943-4F82-BABA-A6D82A9A43C5}">
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{8CF096DE-B943-4F82-BABA-A6D82A9A43C5}">
       <text>
         <r>
           <rPr>
@@ -420,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{E9E07455-9D21-4254-B1CC-9B2704A45D99}">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{E9E07455-9D21-4254-B1CC-9B2704A45D99}">
       <text>
         <r>
           <rPr>
@@ -444,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
+    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
       <text>
         <r>
           <rPr>
@@ -473,7 +498,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="47">
   <si>
     <t>Material</t>
   </si>
@@ -608,6 +633,12 @@
   </si>
   <si>
     <t>rigid.ink Nylon 12</t>
+  </si>
+  <si>
+    <t>Fillamentum CPE HG100</t>
+  </si>
+  <si>
+    <t>Fillamentum CPE HG100 HM100 mod</t>
   </si>
 </sst>
 </file>
@@ -1167,14 +1198,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8993357-4930-402C-A23E-E4B9A1301062}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.140625" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
@@ -1266,34 +1299,34 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>38</v>
@@ -1302,16 +1335,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>38</v>
@@ -1320,16 +1353,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>38</v>
@@ -1338,16 +1371,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>38</v>
@@ -1356,16 +1389,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>38</v>
@@ -1374,16 +1407,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>38</v>
@@ -1392,16 +1425,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>38</v>
@@ -1410,16 +1443,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>38</v>
@@ -1427,32 +1460,32 @@
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>7</v>
@@ -1463,14 +1496,14 @@
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>8</v>
+      <c r="A19" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>7</v>
@@ -1482,88 +1515,88 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="11" t="s">
         <v>41</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>18</v>
+      <c r="C23" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>38</v>
+      <c r="E23" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>38</v>
@@ -1572,16 +1605,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>38</v>
@@ -1589,17 +1622,17 @@
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>25</v>
+      <c r="A26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>38</v>
@@ -1608,43 +1641,61 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C28" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F29" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A5:E28">
-    <sortCondition ref="A5:A28"/>
+  <sortState ref="A5:E29">
+    <sortCondition ref="A5:A29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added details for Proto-pasta PC-ABS filament
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DCA764-4832-474F-A311-03CA545B26FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A6801C-E60E-4049-A3AE-1165D62B5117}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -227,7 +227,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{6FD53F9C-5A10-4655-B410-C14919F7F484}">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{0774A3A8-1D56-4E7B-BD3A-E841559A2162}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darragh Broadbent:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Brim suggested, doesn't seem to work well with the purgebubble method</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{6FD53F9C-5A10-4655-B410-C14919F7F484}">
       <text>
         <r>
           <rPr>
@@ -251,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{7F30C7B6-B556-4FF9-B1F0-6CB901BE9E8C}">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{7F30C7B6-B556-4FF9-B1F0-6CB901BE9E8C}">
       <text>
         <r>
           <rPr>
@@ -275,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{D5CE3906-B1F3-484F-937A-234E258807EE}">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{D5CE3906-B1F3-484F-937A-234E258807EE}">
       <text>
         <r>
           <rPr>
@@ -299,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{E0462C9B-BC3A-4A76-8CFA-B66364D1B3ED}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{E0462C9B-BC3A-4A76-8CFA-B66364D1B3ED}">
       <text>
         <r>
           <rPr>
@@ -323,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{ECE11F64-1683-473C-9AC3-F116D9ED5E60}">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{ECE11F64-1683-473C-9AC3-F116D9ED5E60}">
       <text>
         <r>
           <rPr>
@@ -347,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{0023CEED-8BBE-4786-A3A8-FF9F7051A736}">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{0023CEED-8BBE-4786-A3A8-FF9F7051A736}">
       <text>
         <r>
           <rPr>
@@ -372,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{B0295431-8909-4919-8B34-7A07B2F464CD}">
+    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{B0295431-8909-4919-8B34-7A07B2F464CD}">
       <text>
         <r>
           <rPr>
@@ -397,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="0" shapeId="0" xr:uid="{FA5AB986-6F3D-4095-AA62-83099A764AA8}">
+    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{FA5AB986-6F3D-4095-AA62-83099A764AA8}">
       <text>
         <r>
           <rPr>
@@ -421,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{8CF096DE-B943-4F82-BABA-A6D82A9A43C5}">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{8CF096DE-B943-4F82-BABA-A6D82A9A43C5}">
       <text>
         <r>
           <rPr>
@@ -445,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{E9E07455-9D21-4254-B1CC-9B2704A45D99}">
+    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{E9E07455-9D21-4254-B1CC-9B2704A45D99}">
       <text>
         <r>
           <rPr>
@@ -469,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
       <text>
         <r>
           <rPr>
@@ -498,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
   <si>
     <t>Material</t>
   </si>
@@ -639,6 +663,15 @@
   </si>
   <si>
     <t>Fillamentum CPE HG100 HM100 mod</t>
+  </si>
+  <si>
+    <t>Protopasta PC-ABS</t>
+  </si>
+  <si>
+    <t>Proto-pasta PC-ABS</t>
+  </si>
+  <si>
+    <t>Original Prusa i3 MK3 no purgebubble</t>
   </si>
 </sst>
 </file>
@@ -1198,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8993357-4930-402C-A23E-E4B9A1301062}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,49 +1494,49 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>7</v>
@@ -1514,14 +1547,14 @@
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>8</v>
+      <c r="A20" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>7</v>
@@ -1533,88 +1566,88 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="11" t="s">
         <v>41</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>18</v>
+      <c r="C24" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>38</v>
+      <c r="E24" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>38</v>
@@ -1623,16 +1656,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>38</v>
@@ -1640,17 +1673,17 @@
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>25</v>
+      <c r="A27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>38</v>
@@ -1659,43 +1692,61 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E29" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="5"/>
+      <c r="F30" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A5:E29">
-    <sortCondition ref="A5:A29"/>
+  <sortState ref="A5:E30">
+    <sortCondition ref="A5:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added a number of profiles
Added Taulman PCTPE and Polymaker PolyMax PC profiles, as well as updated material profiles spreadsheet. Updated Proto-pasta PC-ABS profiles
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A6801C-E60E-4049-A3AE-1165D62B5117}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0623F919-9757-4B7A-BA30-C34889307C2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -203,7 +203,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{6CD30595-BA02-485E-9C00-1233A05C83DE}">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{2411A7C2-617C-4578-A4B6-0296745896B9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darragh Broadbent:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Print quality improved by very conservative use of the cooling fan, especially small detail and short layer time, printed with a brim, minimal if any warping.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{6CD30595-BA02-485E-9C00-1233A05C83DE}">
       <text>
         <r>
           <rPr>
@@ -227,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{0774A3A8-1D56-4E7B-BD3A-E841559A2162}">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{0774A3A8-1D56-4E7B-BD3A-E841559A2162}">
       <text>
         <r>
           <rPr>
@@ -251,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{6FD53F9C-5A10-4655-B410-C14919F7F484}">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{6FD53F9C-5A10-4655-B410-C14919F7F484}">
       <text>
         <r>
           <rPr>
@@ -275,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{7F30C7B6-B556-4FF9-B1F0-6CB901BE9E8C}">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{7F30C7B6-B556-4FF9-B1F0-6CB901BE9E8C}">
       <text>
         <r>
           <rPr>
@@ -299,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{D5CE3906-B1F3-484F-937A-234E258807EE}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{D5CE3906-B1F3-484F-937A-234E258807EE}">
       <text>
         <r>
           <rPr>
@@ -323,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{E0462C9B-BC3A-4A76-8CFA-B66364D1B3ED}">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{E0462C9B-BC3A-4A76-8CFA-B66364D1B3ED}">
       <text>
         <r>
           <rPr>
@@ -347,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{ECE11F64-1683-473C-9AC3-F116D9ED5E60}">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{ECE11F64-1683-473C-9AC3-F116D9ED5E60}">
       <text>
         <r>
           <rPr>
@@ -371,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{0023CEED-8BBE-4786-A3A8-FF9F7051A736}">
+    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{0023CEED-8BBE-4786-A3A8-FF9F7051A736}">
       <text>
         <r>
           <rPr>
@@ -396,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{B0295431-8909-4919-8B34-7A07B2F464CD}">
+    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{B0295431-8909-4919-8B34-7A07B2F464CD}">
       <text>
         <r>
           <rPr>
@@ -421,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="0" shapeId="0" xr:uid="{FA5AB986-6F3D-4095-AA62-83099A764AA8}">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{FA5AB986-6F3D-4095-AA62-83099A764AA8}">
       <text>
         <r>
           <rPr>
@@ -445,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{8CF096DE-B943-4F82-BABA-A6D82A9A43C5}">
+    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{8CF096DE-B943-4F82-BABA-A6D82A9A43C5}">
       <text>
         <r>
           <rPr>
@@ -469,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{E9E07455-9D21-4254-B1CC-9B2704A45D99}">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{E9E07455-9D21-4254-B1CC-9B2704A45D99}">
       <text>
         <r>
           <rPr>
@@ -493,7 +517,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
+    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{CE52022A-1191-43A1-BA47-49CAA9AA301B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darragh Broadbent:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not fantastic quality, stringing and warping artifacts, printed with a brim, heavy warping.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
       <text>
         <r>
           <rPr>
@@ -522,7 +570,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="54">
   <si>
     <t>Material</t>
   </si>
@@ -672,6 +720,18 @@
   </si>
   <si>
     <t>Original Prusa i3 MK3 no purgebubble</t>
+  </si>
+  <si>
+    <t>Polymaker PolyMax PC</t>
+  </si>
+  <si>
+    <t>Taulman Alloy 910</t>
+  </si>
+  <si>
+    <t>Polymaker PC-Max fans</t>
+  </si>
+  <si>
+    <t>Taulman PCTPE</t>
   </si>
 </sst>
 </file>
@@ -1231,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8993357-4930-402C-A23E-E4B9A1301062}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,34 +1500,34 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>38</v>
@@ -1476,16 +1536,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>38</v>
@@ -1494,67 +1554,67 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>7</v>
@@ -1565,14 +1625,14 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>8</v>
+      <c r="A21" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>7</v>
@@ -1584,88 +1644,88 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E23" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="11" t="s">
         <v>41</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>18</v>
+      <c r="C25" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>38</v>
+      <c r="E25" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>38</v>
@@ -1674,16 +1734,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>38</v>
@@ -1691,17 +1751,17 @@
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>25</v>
+      <c r="A28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>38</v>
@@ -1710,43 +1770,79 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E30" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F32" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A5:E30">
-    <sortCondition ref="A5:A30"/>
+  <sortState ref="A5:E32">
+    <sortCondition ref="A5:A32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Proto-pasta PC-ABS profile that uses cooling fans
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0623F919-9757-4B7A-BA30-C34889307C2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC9881B-97AF-48FD-A85E-59B7AFA94DAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -271,7 +271,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Brim suggested, doesn't seem to work well with the purgebubble method</t>
+Brim suggested, prints well with the purgebubble method assuming glue stick used on bed.</t>
         </r>
       </text>
     </comment>
@@ -570,7 +570,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="54">
   <si>
     <t>Material</t>
   </si>
@@ -668,9 +668,6 @@
     <t>MK3 Pretty PETG V2 filaprint</t>
   </si>
   <si>
-    <t>Protopasta Conductive</t>
-  </si>
-  <si>
     <t>Proto-pasta HTPLA Matte Fibre</t>
   </si>
   <si>
@@ -713,25 +710,28 @@
     <t>Fillamentum CPE HG100 HM100 mod</t>
   </si>
   <si>
-    <t>Protopasta PC-ABS</t>
-  </si>
-  <si>
     <t>Proto-pasta PC-ABS</t>
   </si>
   <si>
-    <t>Original Prusa i3 MK3 no purgebubble</t>
-  </si>
-  <si>
     <t>Polymaker PolyMax PC</t>
   </si>
   <si>
     <t>Taulman Alloy 910</t>
   </si>
   <si>
-    <t>Polymaker PC-Max fans</t>
-  </si>
-  <si>
     <t>Taulman PCTPE</t>
+  </si>
+  <si>
+    <t>Proto-pasta Conductive</t>
+  </si>
+  <si>
+    <t>Proto-pasta PC-ABS / (fans)</t>
+  </si>
+  <si>
+    <t>Polymaker PC-Max fans / (no fans)</t>
+  </si>
+  <si>
+    <t>Alternate profiles denoted with parentheses</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1294,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1308,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1330,10 +1335,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1350,7 +1355,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="18"/>
     </row>
@@ -1368,49 +1373,49 @@
         <v>20</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
@@ -1422,7 +1427,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1440,7 +1445,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1458,7 +1463,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1476,7 +1481,7 @@
         <v>22</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1494,16 +1499,16 @@
         <v>20</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>52</v>
@@ -1512,7 +1517,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1530,13 +1535,13 @@
         <v>7</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
@@ -1548,43 +1553,43 @@
         <v>22</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1602,7 +1607,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1620,7 +1625,7 @@
         <v>7</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -1638,7 +1643,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1656,7 +1661,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -1674,7 +1679,7 @@
         <v>16</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -1692,25 +1697,25 @@
         <v>7</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -1728,7 +1733,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -1746,7 +1751,7 @@
         <v>22</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -1764,7 +1769,7 @@
         <v>11</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -1782,43 +1787,43 @@
         <v>22</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -1836,7 +1841,7 @@
         <v>23</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F32" s="5"/>
     </row>

</xml_diff>

<commit_message>
Uploaded igus iglidur I180-PF profiles
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2A6BD7-55BB-4A1C-8EB1-6EA0255219D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E6C218-262D-4B68-AB94-F40552F64286}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -106,7 +106,31 @@
     <comment ref="F7" authorId="0" shapeId="0" xr:uid="{221044AA-A390-4D84-BA7C-0914AFFBB821}">
       <text/>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{B2EAE4EC-6C25-4511-9920-3BC8F3F2B3B6}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{99A1B285-34B1-496B-B6DF-B393D3A6FAD3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darragh Broadbent:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Plain PEI bed, also tried glue stick on PEI with mixed results, surface blobbing, easily removed with sharp knife or sandpaper.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{B2EAE4EC-6C25-4511-9920-3BC8F3F2B3B6}">
       <text>
         <r>
           <rPr>
@@ -131,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{A8745309-D847-4CF9-A000-C21A4470BCE6}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{A8745309-D847-4CF9-A000-C21A4470BCE6}">
       <text>
         <r>
           <rPr>
@@ -155,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{985DE15F-4A11-41B1-8852-8A4820DB9028}">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{985DE15F-4A11-41B1-8852-8A4820DB9028}">
       <text>
         <r>
           <rPr>
@@ -179,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{54BD3F34-1376-445B-88F8-B91899B9F727}">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{54BD3F34-1376-445B-88F8-B91899B9F727}">
       <text>
         <r>
           <rPr>
@@ -203,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{2411A7C2-617C-4578-A4B6-0296745896B9}">
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{2411A7C2-617C-4578-A4B6-0296745896B9}">
       <text>
         <r>
           <rPr>
@@ -227,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{6CD30595-BA02-485E-9C00-1233A05C83DE}">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{6CD30595-BA02-485E-9C00-1233A05C83DE}">
       <text>
         <r>
           <rPr>
@@ -251,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{0774A3A8-1D56-4E7B-BD3A-E841559A2162}">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{0774A3A8-1D56-4E7B-BD3A-E841559A2162}">
       <text>
         <r>
           <rPr>
@@ -275,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{6FD53F9C-5A10-4655-B410-C14919F7F484}">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{6FD53F9C-5A10-4655-B410-C14919F7F484}">
       <text>
         <r>
           <rPr>
@@ -299,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{7F30C7B6-B556-4FF9-B1F0-6CB901BE9E8C}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{7F30C7B6-B556-4FF9-B1F0-6CB901BE9E8C}">
       <text>
         <r>
           <rPr>
@@ -323,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{D5CE3906-B1F3-484F-937A-234E258807EE}">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{D5CE3906-B1F3-484F-937A-234E258807EE}">
       <text>
         <r>
           <rPr>
@@ -347,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{E0462C9B-BC3A-4A76-8CFA-B66364D1B3ED}">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{E0462C9B-BC3A-4A76-8CFA-B66364D1B3ED}">
       <text>
         <r>
           <rPr>
@@ -371,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{ECE11F64-1683-473C-9AC3-F116D9ED5E60}">
+    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{ECE11F64-1683-473C-9AC3-F116D9ED5E60}">
       <text>
         <r>
           <rPr>
@@ -395,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{0023CEED-8BBE-4786-A3A8-FF9F7051A736}">
+    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{0023CEED-8BBE-4786-A3A8-FF9F7051A736}">
       <text>
         <r>
           <rPr>
@@ -420,7 +444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{B0295431-8909-4919-8B34-7A07B2F464CD}">
+    <comment ref="D26" authorId="0" shapeId="0" xr:uid="{B0295431-8909-4919-8B34-7A07B2F464CD}">
       <text>
         <r>
           <rPr>
@@ -445,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{FA5AB986-6F3D-4095-AA62-83099A764AA8}">
+    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{FA5AB986-6F3D-4095-AA62-83099A764AA8}">
       <text>
         <r>
           <rPr>
@@ -469,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{8CF096DE-B943-4F82-BABA-A6D82A9A43C5}">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{8CF096DE-B943-4F82-BABA-A6D82A9A43C5}">
       <text>
         <r>
           <rPr>
@@ -493,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{E9E07455-9D21-4254-B1CC-9B2704A45D99}">
+    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{E9E07455-9D21-4254-B1CC-9B2704A45D99}">
       <text>
         <r>
           <rPr>
@@ -517,7 +541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{CE52022A-1191-43A1-BA47-49CAA9AA301B}">
+    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{CE52022A-1191-43A1-BA47-49CAA9AA301B}">
       <text>
         <r>
           <rPr>
@@ -541,7 +565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
+    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
       <text>
         <r>
           <rPr>
@@ -570,7 +594,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
   <si>
     <t>Material</t>
   </si>
@@ -671,12 +695,6 @@
     <t>Fillamentum PLA Extrafill</t>
   </si>
   <si>
-    <t>igus iglidur I150</t>
-  </si>
-  <si>
-    <t>iglidur I150</t>
-  </si>
-  <si>
     <t>Enclosure used</t>
   </si>
   <si>
@@ -732,6 +750,18 @@
   </si>
   <si>
     <t>PrusaSlicer profiles</t>
+  </si>
+  <si>
+    <t>iglidur I180-PF</t>
+  </si>
+  <si>
+    <t>igus iglidur I180-PF</t>
+  </si>
+  <si>
+    <t>iglidur I150-PF</t>
+  </si>
+  <si>
+    <t>igus iglidur I150-PF</t>
   </si>
 </sst>
 </file>
@@ -1291,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8993357-4930-402C-A23E-E4B9A1301062}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,17 +1338,17 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1335,10 +1365,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1355,7 +1385,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="18"/>
     </row>
@@ -1373,481 +1403,499 @@
         <v>19</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>44</v>
+        <v>53</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>18</v>
+        <v>45</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="E20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>4</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
+      <c r="A22" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="E24" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>42</v>
+        <v>20</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>39</v>
+      <c r="E25" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>17</v>
+      <c r="C26" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>36</v>
+      <c r="E26" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="E29" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>41</v>
+        <v>24</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>39</v>
+        <v>21</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>48</v>
+        <v>6</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="D31" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+      <c r="E32" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" s="5"/>
+      <c r="E33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A5:E32">
-    <sortCondition ref="A5:A32"/>
+  <sortState ref="A5:E33">
+    <sortCondition ref="A5:A33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded profiles for Verbatim PP and Primalloy
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Darragh\Documents\GitHub\Prusa-MK3-Material-Profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E6C218-262D-4B68-AB94-F40552F64286}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47087818-4D73-458D-8EF7-C82572D950FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73692AA3-BA34-4172-88CE-EEE2FFA9ADF6}"/>
   </bookViews>
@@ -565,7 +565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
+    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{13B6180B-A46B-461F-B864-D5C480D439DE}">
       <text>
         <r>
           <rPr>
@@ -586,6 +586,55 @@
           </rPr>
           <t xml:space="preserve">
 Standard Slic3r profile for T-Glase is nonsense, bed temperature above the glass transition for the material? ¯\_(ツ)_/¯ Generated new profile using guidance from Taulman, and a bit of trial and error</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0" shapeId="0" xr:uid="{F29BC682-E3C6-4621-BC5C-D502A26D9926}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Darragh Broadbent:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Brim suggested, packing tape on bed.
+Changes made to the normal Prusa profile are just speeds, original a bit too fast.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D35" authorId="0" shapeId="0" xr:uid="{A6EF5D67-670B-4DD4-81DA-A5F98F3CB0C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Darragh Broadbent:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Stringy, surface blobbing, not a great result</t>
         </r>
       </text>
     </comment>
@@ -594,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="59">
   <si>
     <t>Material</t>
   </si>
@@ -762,6 +811,15 @@
   </si>
   <si>
     <t>igus iglidur I150-PF</t>
+  </si>
+  <si>
+    <t>Verbatim Primalloy</t>
+  </si>
+  <si>
+    <t>Verbatim PP</t>
+  </si>
+  <si>
+    <t>Verbatim PP mod</t>
   </si>
 </sst>
 </file>
@@ -819,7 +877,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -846,17 +904,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -948,17 +995,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -985,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -996,17 +1032,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1321,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8993357-4930-402C-A23E-E4B9A1301062}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1370,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1352,550 +1385,586 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="19"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>37</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A5:E33">
-    <sortCondition ref="A5:A33"/>
+  <sortState ref="A5:E35">
+    <sortCondition ref="A5:A35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added info for 3DJake Skulpt
Added 3DJake Skulpt profile info to spreadsheet, added a low first layer speed 0.15mm QUALITY MK3 profile as well.
</commit_message>
<xml_diff>
--- a/materialprofiles.xlsx
+++ b/materialprofiles.xlsx
@@ -7,6 +7,11 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhXHF4op4WmQCeN4Sj9ZHyP4jlqAA=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -18,179 +23,241 @@
   <commentList>
     <comment authorId="0" ref="D5">
       <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Prints good, colour not nearly as vivid when compared to rigid.ink, I have only used orange. </t>
+        <t xml:space="preserve">======
+ID#AAAAI98E4AQ
+Darragh Broadbent    (2020-02-21 13:50:35)
+Prints reasonably well, a little messy on overhangs and bridging. Slight warping.</t>
       </text>
     </comment>
     <comment authorId="0" ref="D6">
       <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Quite stringy, moreso that the Polywood</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D7">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Stringy but cleans up fine.
-</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D8">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Plain PEI bed, also tried glue stick on PEI with mixed results, surface blobbing, easily removed with sharp knife or sandpaper.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D9">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-First print came out really well, I have just changed things like minimum speeds and minimum layer times to improve reliability. No brim used but slight warping was seen on Benchy base.
-</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D11">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent
-Brim suggested, slight warping on base. Magigoo PP used on bed, almost no stringing. Potentially overcooled on some layers.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D13">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-A very small amount of discolouration on one of the pillars</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D14">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Slight artifacts on overhangs</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D15">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-A little stringy</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D16">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Print quality improved by very conservative use of the cooling fan, especially small detail and short layer time, printed with a brim, minimal if any warping. Layer of glue stick on bed.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D19">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-First layer 240°C to break nozzle blockage, further layers 210, could potentially go lower.
-</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D20">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Consistent, light stringing, first layer 240°C to break nozzle blockage, further layers 210, could potentially go lower.
-</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D21">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
+        <t xml:space="preserve">======
+ID#AAAAI98E4AI
+Darragh Broadbent    (2020-02-21 13:47:53)
+Prints good, colour not nearly as vivid when compared to rigid.ink, I have only used orange.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D22">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAo
+Darragh Broadbent    (2020-02-21 12:10:25)
 Brim suggested, prints well with the purgebubble method assuming glue stick used on bed. A significant decrease in layer to layer strength is in evidence with fans engaged, use with caution.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D22">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Quite oozy, used gluestick on PEI bed?</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D23">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Turn overhangs towards the front of the printer. (into wind as far as the part cooling fan is concerned) Pretty happy with print quality now, brim helpful.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D24">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Turn overhangs towards the front of the printer. (into wind as far as the part cooling fan is concerned) Pretty happy with print quality now. Dry filament before usage. Brim helpful.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D25">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Turn overhangs towards the front of the printer. (into wind as far as the part cooling fan is concerned) Pretty happy with print quality now. Brim helpful</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D26">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Unhappy with print quality, quite oozey, to be revisited.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D27">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Print quality now quite good, brim helpful
-</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D28">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Reasonably happy with print quality, brim helpful. Dry filament before use.
-</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D31">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Unhappy with print quality, to be revisited.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D32">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Tiny amounts of stringyness, used gluestick on PEI bed</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D33">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Tiny bit of stringing, thin layer of glue stick required, bridging not wonderful. Dry filament before use.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D34">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Not fantastic quality, stringing and warping artifacts, printed with a brim, heavy warping. Glue stick on bed.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D35">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
-Standard Slic3r profile for T-Glase is nonsense, bed temperature above the glass transition for the material? ¯\_(ツ)_/¯ Generated new profile using guidance from Taulman, and a bit of trial and error</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D36">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
+    <comment authorId="0" ref="D37">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAk
+Darragh Broadbent    (2020-02-21 12:10:25)
 Brim suggested, packing tape on bed.
 Changes made to the normal Prusa profile are just speeds, original a bit too fast.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D37">
-      <text>
-        <t xml:space="preserve">Darragh Broadbent:
+    <comment authorId="0" ref="D28">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAg
+Darragh Broadbent    (2020-02-21 12:10:25)
+Print quality now quite good, brim helpful</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D23">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAc
+Darragh Broadbent    (2020-02-21 12:10:25)
+Quite oozy, used gluestick on PEI bed?</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D8">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAY
+Darragh Broadbent    (2020-02-21 12:10:25)
+Stringy but cleans up fine.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D25">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAU
+Darragh Broadbent    (2020-02-21 12:10:25)
+Turn overhangs towards the front of the printer. (into wind as far as the part cooling fan is concerned) Pretty happy with print quality now. Dry filament before usage. Brim helpful.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D17">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAQ
+Darragh Broadbent    (2020-02-21 12:10:25)
+Print quality improved by very conservative use of the cooling fan, especially small detail and short layer time, printed with a brim, minimal if any warping. Layer of glue stick on bed.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D12">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAM
+    (2020-02-21 12:10:25)
+Darragh Broadbent
+Brim suggested, slight warping on base. Magigoo PP used on bed, almost no stringing. Potentially overcooled on some layers.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D32">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAI
+Darragh Broadbent    (2020-02-21 12:10:25)
+Unhappy with print quality, to be revisited.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D15">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TzAE
+Darragh Broadbent    (2020-02-21 12:10:25)
+Slight artifacts on overhangs</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D33">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvEU
+Darragh Broadbent    (2020-02-21 12:10:25)
+Tiny amounts of stringyness, used gluestick on PEI bed</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D20">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvEQ
+Darragh Broadbent    (2020-02-21 12:10:25)
+First layer 240°C to break nozzle blockage, further layers 210, could potentially go lower.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D9">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvEM
+Darragh Broadbent    (2020-02-21 12:10:25)
+Plain PEI bed, also tried glue stick on PEI with mixed results, surface blobbing, easily removed with sharp knife or sandpaper.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D29">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvEI
+Darragh Broadbent    (2020-02-21 12:10:25)
+Reasonably happy with print quality, brim helpful. Dry filament before use.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D26">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvEE
+Darragh Broadbent    (2020-02-21 12:10:25)
+Turn overhangs towards the front of the printer. (into wind as far as the part cooling fan is concerned) Pretty happy with print quality now. Brim helpful</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D34">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvEA
+Darragh Broadbent    (2020-02-21 12:10:25)
+Tiny bit of stringing, thin layer of glue stick required, bridging not wonderful. Dry filament before use.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D36">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvD8
+Darragh Broadbent    (2020-02-21 12:10:25)
+Standard Slic3r profile for T-Glase is nonsense, bed temperature above the glass transition for the material? ¯\_(ツ)_/¯ Generated new profile using guidance from Taulman, and a bit of trial and error</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D35">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvD0
+Darragh Broadbent    (2020-02-21 12:10:25)
+Not fantastic quality, stringing and warping artifacts, printed with a brim, heavy warping. Glue stick on bed.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D38">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvDw
+Darragh Broadbent    (2020-02-21 12:10:25)
 Stringy, surface blobbing, not a great result</t>
       </text>
     </comment>
+    <comment authorId="0" ref="D24">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvDs
+Darragh Broadbent    (2020-02-21 12:10:25)
+Turn overhangs towards the front of the printer. (into wind as far as the part cooling fan is concerned) Pretty happy with print quality now, brim helpful.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D21">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvDo
+Darragh Broadbent    (2020-02-21 12:10:25)
+Consistent, light stringing, first layer 240°C to break nozzle blockage, further layers 210, could potentially go lower.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D27">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvDk
+Darragh Broadbent    (2020-02-21 12:10:25)
+Unhappy with print quality, quite oozey, to be revisited.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D7">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvDg
+Darragh Broadbent    (2020-02-21 12:10:25)
+Quite stringy, moreso that the Polywood</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D16">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvDc
+Darragh Broadbent    (2020-02-21 12:10:25)
+A little stringy</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D14">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvDY
+Darragh Broadbent    (2020-02-21 12:10:25)
+A very small amount of discolouration on one of the pillars</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D10">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAJI7TvDU
+Darragh Broadbent    (2020-02-21 12:10:25)
+First print came out really well, I have just changed things like minimum speeds and minimum layer times to improve reliability. No brim used but slight warping was seen on Benchy base.</t>
+      </text>
+    </comment>
   </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mg2suH7ZZahbD3ibmH8lpLTan6+jg=="/>
+    </ext>
+  </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="64">
   <si>
     <t>READ THE NOTES IN COLUMN D</t>
   </si>
@@ -219,16 +286,25 @@
     <t>Images (roll over to view)</t>
   </si>
   <si>
+    <t>3DJake Skulpt</t>
+  </si>
+  <si>
+    <t>0.15 QUALITY MK3 slow first layer</t>
+  </si>
+  <si>
+    <t>Prusament PLA</t>
+  </si>
+  <si>
+    <t>Original Prusa i3 MK3 purgebubble</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Amazonbasics PLA</t>
   </si>
   <si>
     <t>rigid.ink PLA</t>
-  </si>
-  <si>
-    <t>Original Prusa i3 MK3 purgebubble</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Easywood PLA</t>
@@ -379,7 +455,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -398,6 +474,15 @@
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -511,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -521,11 +606,35 @@
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -750,7 +859,6 @@
     <col customWidth="1" min="3" max="3" width="29.38"/>
     <col customWidth="1" min="4" max="5" width="28.13"/>
     <col customWidth="1" min="6" max="6" width="21.0"/>
-    <col customWidth="1" min="7" max="26" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -789,602 +897,641 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="18"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="C24" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="s">
+      <c r="E31" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="E33" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="9" t="s">
+      <c r="E35" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="11"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F34" s="11"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="11"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" s="11"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="15"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1"/>
+      <c r="E37" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="23"/>
+    </row>
     <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="2"/>
+    </row>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1"/>
@@ -2345,6 +2492,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>